<commit_message>
Shadows on cell text are not supported. Remove it from the test. Shadows are supported only on textboxes and shapes.
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/Styles/StyleFont.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/Styles/StyleFont.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <x:si>
     <x:t>Bold</x:t>
   </x:si>
@@ -32,9 +32,6 @@
   </x:si>
   <x:si>
     <x:t>Italic - true</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Shadow - true</x:t>
   </x:si>
   <x:si>
     <x:t>Strikethrough - true</x:t>
@@ -53,7 +50,7 @@
   <x:numFmts count="1">
     <x:numFmt numFmtId="0" formatCode=""/>
   </x:numFmts>
-  <x:fonts count="11">
+  <x:fonts count="10">
     <x:font>
       <x:vertAlign val="baseline"/>
       <x:sz val="11"/>
@@ -100,14 +97,6 @@
     <x:font>
       <x:i/>
       <x:vertAlign val="baseline"/>
-      <x:sz val="11"/>
-      <x:color rgb="FF000000"/>
-      <x:name val="Calibri"/>
-      <x:family val="2"/>
-    </x:font>
-    <x:font>
-      <x:vertAlign val="baseline"/>
-      <x:shadow/>
       <x:sz val="11"/>
       <x:color rgb="FF000000"/>
       <x:name val="Calibri"/>
@@ -164,7 +153,7 @@
       </x:diagonal>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="11">
+  <x:cellStyleXfs count="10">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -195,11 +184,8 @@
     <x:xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="11">
+  <x:cellXfs count="10">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
@@ -237,10 +223,6 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -539,7 +521,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:B11"/>
+  <x:dimension ref="A1:B10"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -580,7 +562,7 @@
       </x:c>
     </x:row>
     <x:row r="8" spans="1:2">
-      <x:c r="B8" s="0" t="s">
+      <x:c r="B8" s="7" t="s">
         <x:v>6</x:v>
       </x:c>
     </x:row>
@@ -592,11 +574,6 @@
     <x:row r="10" spans="1:2">
       <x:c r="B10" s="9" t="s">
         <x:v>8</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="11" spans="1:2">
-      <x:c r="B11" s="10" t="s">
-        <x:v>9</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Add support for setting charset
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/Styles/StyleFont.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/Styles/StyleFont.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <x:si>
     <x:t>Bold</x:t>
   </x:si>
@@ -23,6 +23,9 @@
   </x:si>
   <x:si>
     <x:t>FontFamilyNumbering - Script</x:t>
+  </x:si>
+  <x:si>
+    <x:t>FontCharSet - العربية التنضيد</x:t>
   </x:si>
   <x:si>
     <x:t>FontName - Stencil</x:t>
@@ -50,7 +53,7 @@
   <x:numFmts count="1">
     <x:numFmt numFmtId="0" formatCode=""/>
   </x:numFmts>
-  <x:fonts count="10">
+  <x:fonts count="11">
     <x:font>
       <x:vertAlign val="baseline"/>
       <x:sz val="11"/>
@@ -79,6 +82,14 @@
       <x:color rgb="FF000000"/>
       <x:name val="Calibri"/>
       <x:family val="4"/>
+    </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Arabic Typesetting"/>
+      <x:family val="2"/>
+      <x:charset val="178"/>
     </x:font>
     <x:font>
       <x:vertAlign val="baseline"/>
@@ -153,7 +164,7 @@
       </x:diagonal>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="10">
+  <x:cellStyleXfs count="11">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -184,8 +195,11 @@
     <x:xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="10">
+  <x:cellXfs count="11">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
@@ -223,6 +237,10 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -521,7 +539,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:B10"/>
+  <x:dimension ref="A1:B11"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -576,6 +594,11 @@
         <x:v>8</x:v>
       </x:c>
     </x:row>
+    <x:row r="11" spans="1:2">
+      <x:c r="B11" s="10" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>